<commit_message>
doc: update wo spreadsheet
</commit_message>
<xml_diff>
--- a/app/docs/wohin_wo_woher.xlsx
+++ b/app/docs/wohin_wo_woher.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javen\Development\react-redux\app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDFF4B6-8ACE-4F0A-9D0D-0D6844DFF138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6E537-C3B5-4B7A-9EE5-BA7FE166DBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{5F88E16C-B0F0-4698-8527-E7CEDE9EB5AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -813,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B931BE20-ABFB-498A-9F37-4777EBF1D3C9}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>